<commit_message>
Deploying to gh-pages from  @ 6e061cf8710fa5ad40cf5074917b504e626746ec 🚀
</commit_message>
<xml_diff>
--- a/en/downloads/data-excel/12.4.2.xlsx
+++ b/en/downloads/data-excel/12.4.2.xlsx
@@ -209,7 +209,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -260,10 +260,19 @@
     <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -575,7 +584,7 @@
   <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,25 +665,25 @@
       <c r="C4" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="21">
         <v>136.80000000000001</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="22">
         <v>10455.799999999999</v>
       </c>
-      <c r="F4" s="14">
+      <c r="F4" s="22">
         <v>12332.6</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="22">
         <v>12610.3</v>
       </c>
-      <c r="H4" s="14">
+      <c r="H4" s="22">
         <v>12002.6</v>
       </c>
-      <c r="I4" s="14">
+      <c r="I4" s="22">
         <v>11223.2</v>
       </c>
-      <c r="J4" s="19">
+      <c r="J4" s="18">
         <v>11545.7</v>
       </c>
     </row>
@@ -688,26 +697,26 @@
       <c r="C5" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="14">
+      <c r="D5" s="22">
         <v>5895.1</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="22">
         <v>6019.5</v>
       </c>
-      <c r="F5" s="14">
+      <c r="F5" s="22">
         <v>6140.2</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="22">
         <v>6256.7</v>
       </c>
-      <c r="H5" s="14">
+      <c r="H5" s="22">
         <v>6389.5</v>
       </c>
-      <c r="I5" s="14">
+      <c r="I5" s="22">
         <v>6523.5</v>
       </c>
-      <c r="J5" s="18" t="s">
-        <v>15</v>
+      <c r="J5" s="19">
+        <v>6636.8</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="27" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -739,8 +748,8 @@
         <f>I4/I5*1000</f>
         <v>1720.4261516057334</v>
       </c>
-      <c r="J6" s="17">
-        <v>6636.8</v>
+      <c r="J6" s="20" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">

</xml_diff>